<commit_message>
vault backup: 2025-04-02 09:52:49
</commit_message>
<xml_diff>
--- a/trips/Money_calultor.xlsx
+++ b/trips/Money_calultor.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\trips\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439DE5FD-628F-4856-9203-74D3BD067363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F79F2E4-E710-4B8F-82A6-7207F6FCB834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4DD1103-9CC4-4D40-83CE-CC03A5B21616}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B4DD1103-9CC4-4D40-83CE-CC03A5B21616}"/>
   </bookViews>
   <sheets>
     <sheet name="房费" sheetId="1" r:id="rId1"/>
     <sheet name="账号" sheetId="2" r:id="rId2"/>
     <sheet name="其他门票" sheetId="3" r:id="rId3"/>
+    <sheet name="Yang" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>M Ren</t>
   </si>
@@ -82,6 +83,15 @@
   <si>
     <t>Camping de Rimboe info@campingderimboe.com
 Telefoon: +31 (0)318482371</t>
+  </si>
+  <si>
+    <t>aosiwei</t>
+  </si>
+  <si>
+    <t>130plz</t>
+  </si>
+  <si>
+    <t>mine</t>
   </si>
 </sst>
 </file>
@@ -197,30 +207,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF67E85-D6B6-400D-ACBE-5DCC7495CB9E}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,38 +575,36 @@
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
         <v>25.95</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3">
         <v>25.95</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <f>C3/2</f>
         <v>12.975</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -623,51 +630,50 @@
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>287.97000000000003</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <f>B7/3</f>
         <v>95.990000000000009</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>95.990000000000009</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7">
         <v>95.990000000000009</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <f>C7/6</f>
         <v>15.998333333333335</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <f>D7/6</f>
         <v>15.998333333333335</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <f>E7/5</f>
         <v>19.198</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -685,34 +691,31 @@
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6">
+      <c r="D11">
         <v>756</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11">
         <v>756</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <f>E11/6</f>
         <v>126</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -738,50 +741,46 @@
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
+      <c r="E15">
         <v>380.87</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15">
         <f>E15/2</f>
         <v>190.435</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15">
         <v>190.435</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <f>F15/6</f>
         <v>31.739166666666666</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="7">
         <f>G15/5</f>
         <v>38.087000000000003</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -828,4 +827,35 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6529ABC6-1F05-4970-B03D-F5BDC8CE7623}">
+  <dimension ref="C2:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-09-15 15:00:46
</commit_message>
<xml_diff>
--- a/trips/Money_calultor.xlsx
+++ b/trips/Money_calultor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\trips\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F79F2E4-E710-4B8F-82A6-7207F6FCB834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E0F9E0-8E22-48C8-88A7-16398212DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B4DD1103-9CC4-4D40-83CE-CC03A5B21616}"/>
+    <workbookView xWindow="2895" yWindow="150" windowWidth="25500" windowHeight="15345" xr2:uid="{B4DD1103-9CC4-4D40-83CE-CC03A5B21616}"/>
   </bookViews>
   <sheets>
     <sheet name="房费" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>M Ren</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>mine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">单人 </t>
+  </si>
+  <si>
+    <t>（已修改，不再有效）</t>
+  </si>
+  <si>
+    <t>已经收钱</t>
+  </si>
+  <si>
+    <t>差价</t>
+  </si>
+  <si>
+    <t>建敏需转给个人差价</t>
   </si>
 </sst>
 </file>
@@ -107,12 +122,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -207,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -230,6 +251,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,20 +604,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF67E85-D6B6-400D-ACBE-5DCC7495CB9E}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3">
@@ -571,7 +631,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -587,7 +647,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -606,8 +666,8 @@
       <c r="G4" s="12"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3">
@@ -626,7 +686,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -649,7 +709,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -675,8 +735,8 @@
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -687,7 +747,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -699,7 +759,7 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
@@ -717,76 +777,215 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16">
         <v>45139</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="16">
         <v>45505</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
+      <c r="H14" s="15"/>
+      <c r="I14" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="J14" s="15"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E15">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19">
         <v>380.87</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="19">
         <f>E15/2</f>
         <v>190.435</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="19">
         <v>190.435</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="H15" s="19"/>
+      <c r="I15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
+      <c r="L15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="23">
         <f>F15/6</f>
         <v>31.739166666666666</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="23">
         <f>G15/5</f>
         <v>38.087000000000003</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="13"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="25"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28">
+        <v>45139</v>
+      </c>
+      <c r="G19" s="28">
+        <v>45505</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="27"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34">
+        <v>175.46</v>
+      </c>
+      <c r="G20" s="34">
+        <v>119.82</v>
+      </c>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="35"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="34">
+        <f>F20/6</f>
+        <v>29.243333333333336</v>
+      </c>
+      <c r="G21" s="34">
+        <f>G20/4</f>
+        <v>29.954999999999998</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34">
+        <v>35.1</v>
+      </c>
+      <c r="G22" s="34">
+        <v>39.94</v>
+      </c>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="36"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="34">
+        <f>F22*5</f>
+        <v>175.5</v>
+      </c>
+      <c r="G23" s="34">
+        <f>G22*3</f>
+        <v>119.82</v>
+      </c>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="36"/>
+    </row>
+    <row r="24" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="33">
+        <f>F22-F21</f>
+        <v>5.8566666666666656</v>
+      </c>
+      <c r="G24" s="33">
+        <f>G22-G21</f>
+        <v>9.9849999999999994</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="G7:I8"/>
     <mergeCell ref="I15:K16"/>
     <mergeCell ref="F3:H4"/>
+    <mergeCell ref="I20:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -833,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6529ABC6-1F05-4970-B03D-F5BDC8CE7623}">
   <dimension ref="C2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>